<commit_message>
adicionado criterio de cidade grande, media e pequenas
</commit_message>
<xml_diff>
--- a/output/flourish_prefeitos_municipios_densidade.xlsx
+++ b/output/flourish_prefeitos_municipios_densidade.xlsx
@@ -703,10 +703,10 @@
         <v>126</v>
       </c>
       <c r="E16">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="F16">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -720,13 +720,13 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E17">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F17">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -743,10 +743,10 @@
         <v>274</v>
       </c>
       <c r="E18">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="F18">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -760,13 +760,13 @@
         <v>3</v>
       </c>
       <c r="D19">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E19">
-        <v>976</v>
+        <v>979</v>
       </c>
       <c r="F19">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -780,13 +780,13 @@
         <v>4</v>
       </c>
       <c r="D20">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E20">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F20">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -800,13 +800,13 @@
         <v>5</v>
       </c>
       <c r="D21">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E21">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F21">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -820,13 +820,13 @@
         <v>6</v>
       </c>
       <c r="D22">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E22">
         <v>209</v>
       </c>
       <c r="F22">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -840,10 +840,10 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F23">
         <v>91</v>
@@ -860,10 +860,10 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E24">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F24">
         <v>82</v>
@@ -880,13 +880,13 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E25">
         <v>666</v>
       </c>
       <c r="F25">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -900,13 +900,13 @@
         <v>3</v>
       </c>
       <c r="D26">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E26">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="F26">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -923,10 +923,10 @@
         <v>218</v>
       </c>
       <c r="E27">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F27">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -940,10 +940,10 @@
         <v>5</v>
       </c>
       <c r="D28">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F28">
         <v>55</v>
@@ -960,10 +960,10 @@
         <v>6</v>
       </c>
       <c r="D29">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E29">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F29">
         <v>37</v>
@@ -980,10 +980,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E30">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F30">
         <v>106</v>
@@ -1003,10 +1003,10 @@
         <v>127</v>
       </c>
       <c r="E31">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F31">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1020,13 +1020,13 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E32">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="F32">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:6">

</xml_diff>